<commit_message>
Updated excel sheet with DB details.
</commit_message>
<xml_diff>
--- a/docs/DB_tables.xlsx
+++ b/docs/DB_tables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t>Dtype:</t>
   </si>
@@ -120,6 +120,9 @@
     <t>JSON from ALAMUT</t>
   </si>
   <si>
+    <t>?</t>
+  </si>
+  <si>
     <t>Info from Alamut (split or enter as JSON?)</t>
   </si>
   <si>
@@ -136,6 +139,33 @@
   </si>
   <si>
     <t>reference allele base</t>
+  </si>
+  <si>
+    <t>Type of panel (e.g. APN, HSP, Filtex, Exome, ALS)</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>Varchar</t>
+  </si>
+  <si>
+    <t>e.g. 1995</t>
+  </si>
+  <si>
+    <t>e.g. 432_13</t>
+  </si>
+  <si>
+    <t>varchar?</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>F/M</t>
+  </si>
+  <si>
+    <t>Float</t>
   </si>
 </sst>
 </file>
@@ -513,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -553,46 +583,68 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="F8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>15</v>
+      <c r="C9" t="s">
+        <v>42</v>
       </c>
       <c r="F9" t="s">
         <v>35</v>
@@ -600,7 +652,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
       </c>
       <c r="F10" t="s">
         <v>36</v>
@@ -608,84 +663,122 @@
     </row>
     <row r="11" spans="1:6">
       <c r="B11" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="F12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>29</v>
       </c>
-      <c r="F17" t="s">
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="B18" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="B19" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="B21" t="s">
         <v>32</v>
       </c>
-      <c r="F20" t="s">
+      <c r="C21" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" t="s">
+      <c r="F21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
         <v>20</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>21</v>
       </c>
-      <c r="F25" t="s">
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="B26" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="B27" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="B28" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="B30" t="s">
         <v>27</v>
+      </c>
+      <c r="C30" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some files (hsmetrics)
</commit_message>
<xml_diff>
--- a/docs/DB_tables.xlsx
+++ b/docs/DB_tables.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
   <si>
     <t>Dtype:</t>
   </si>
@@ -39,15 +39,9 @@
     <t>Patient_info</t>
   </si>
   <si>
-    <t>Patient ID</t>
-  </si>
-  <si>
     <t>Birthyear</t>
   </si>
   <si>
-    <t>Clinical information</t>
-  </si>
-  <si>
     <t>Family ID</t>
   </si>
   <si>
@@ -60,9 +54,6 @@
     <t>Info/comments</t>
   </si>
   <si>
-    <t>Seq_variants</t>
-  </si>
-  <si>
     <t>Chr</t>
   </si>
   <si>
@@ -105,9 +96,6 @@
     <t>% X &gt; 30 X</t>
   </si>
   <si>
-    <t>% of targeted bases have a higher than 20 X coverage</t>
-  </si>
-  <si>
     <t>Class</t>
   </si>
   <si>
@@ -166,13 +154,61 @@
   </si>
   <si>
     <t>Float</t>
+  </si>
+  <si>
+    <t>Users:</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>Panels:</t>
+  </si>
+  <si>
+    <t>Fkey - panels</t>
+  </si>
+  <si>
+    <t>Type panel</t>
+  </si>
+  <si>
+    <t>pv2-1, exom, filtex</t>
+  </si>
+  <si>
+    <t>Patient_ID</t>
+  </si>
+  <si>
+    <t>Clinical_info</t>
+  </si>
+  <si>
+    <t>raw_variants</t>
+  </si>
+  <si>
+    <t>hg</t>
+  </si>
+  <si>
+    <t>hg19</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>QC:</t>
+  </si>
+  <si>
+    <t>info fra Hsmetrics (JSON?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -184,6 +220,22 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -206,14 +258,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Fulgt hyperkobling" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Fulgt hyperkobling" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperkobling" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -543,16 +615,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
     <col min="6" max="6" width="44.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -573,7 +646,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -581,208 +654,276 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>37</v>
+      </c>
+      <c r="F20" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="B21" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="B26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="B27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" t="s">
-        <v>24</v>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>38</v>
+      </c>
+      <c r="D28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="B29" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" t="s">
         <v>48</v>
       </c>
-      <c r="F29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="B30" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="36" spans="1:4">
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="B43" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="B44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="B45" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated table schema and added a file containing info for filling db with example data
</commit_message>
<xml_diff>
--- a/docs/DB_tables.xlsx
+++ b/docs/DB_tables.xlsx
@@ -327,10 +327,10 @@
     <t>alt</t>
   </si>
   <si>
-    <t>variant_annotation</t>
-  </si>
-  <si>
     <t>interpretations</t>
+  </si>
+  <si>
+    <t>alamut_annotation</t>
   </si>
 </sst>
 </file>
@@ -768,7 +768,7 @@
   <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B14" sqref="B14:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -984,7 +984,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
@@ -1022,7 +1022,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
         <v>14</v>

</xml_diff>